<commit_message>
[SHUBHAM] Add new ChromeDriver
</commit_message>
<xml_diff>
--- a/data/excel/FlightBookingWithMoreProducts.xlsx
+++ b/data/excel/FlightBookingWithMoreProducts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9ED93-5022-401A-A23E-2EA4FAD94354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5BF1B3-45CB-4818-ADBA-6B385D72E1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8512" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8888" uniqueCount="588">
   <si>
     <t>del</t>
   </si>
@@ -1780,6 +1780,45 @@
   </si>
   <si>
     <t>Flight+MoreProducts</t>
+  </si>
+  <si>
+    <t>Mumbai, India - Shivaji Terminal (BOM)</t>
+  </si>
+  <si>
+    <t>Mumbai, India - Mumbai - Airport</t>
+  </si>
+  <si>
+    <t>New Delhi, India - New Delhi - Airport</t>
+  </si>
+  <si>
+    <t>13B,5E,6D,12E</t>
+  </si>
+  <si>
+    <t>HotelsOnRequest,SelfDriveCar,Insurance,Bus</t>
+  </si>
+  <si>
+    <t>ComplexItineraryAir,Forex,Visa,Insurance,Bus,Rail</t>
+  </si>
+  <si>
+    <t>Visa,Insurance</t>
+  </si>
+  <si>
+    <t>Visa,Insurance,Bus</t>
+  </si>
+  <si>
+    <t>Verify on Add to Cart with adding 8 more products for Flight booking.</t>
+  </si>
+  <si>
+    <t>Verify on Add to Cart with adding 4 more products for Flight booking.</t>
+  </si>
+  <si>
+    <t>Verify on Add to Cart with adding 6 more products for Flight booking.</t>
+  </si>
+  <si>
+    <t>Verify on Add to Cart with adding 2 more products for Flight booking.</t>
+  </si>
+  <si>
+    <t>Verify on Add to Cart with adding 3 more products for Flight booking.</t>
   </si>
 </sst>
 </file>
@@ -19060,16 +19099,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1152101-88D1-47D8-974F-BB578AD00182}">
-  <dimension ref="A1:DG2"/>
+  <dimension ref="A1:DG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BB7" sqref="BB7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
@@ -19117,7 +19156,7 @@
     <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
@@ -19127,7 +19166,7 @@
     <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="9" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="13.85546875" customWidth="1"/>
     <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="11" bestFit="1" customWidth="1"/>
@@ -19520,7 +19559,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>500</v>
+        <v>583</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>56</v>
@@ -19595,10 +19634,10 @@
         <v>246</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>69</v>
@@ -19694,10 +19733,10 @@
         <v>4</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>484</v>
+        <v>448</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>33</v>
+        <v>575</v>
       </c>
       <c r="BJ2" s="1">
         <v>1</v>
@@ -19709,13 +19748,13 @@
         <v>559</v>
       </c>
       <c r="BM2" s="1" t="s">
-        <v>560</v>
+        <v>576</v>
       </c>
       <c r="BN2" s="1" t="s">
         <v>561</v>
       </c>
       <c r="BO2" s="1" t="s">
-        <v>562</v>
+        <v>577</v>
       </c>
       <c r="BP2" s="1" t="s">
         <v>411</v>
@@ -19838,7 +19877,7 @@
         <v>153</v>
       </c>
       <c r="DD2" s="7" t="s">
-        <v>304</v>
+        <v>578</v>
       </c>
       <c r="DE2" s="7" t="s">
         <v>145</v>
@@ -19850,141 +19889,1482 @@
         <v>432</v>
       </c>
     </row>
+    <row r="3" spans="1:111" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB3" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC3" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE3" s="38" t="s">
+        <v>579</v>
+      </c>
+      <c r="BF3" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="BG3" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI3" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK3" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO3" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BP3" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BQ3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="BR3" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS3" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="BU3" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY3" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BZ3" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CA3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB3" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="CC3" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CJ3" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="CK3" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="CM3" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="CN3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="CO3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="CQ3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="CR3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CU3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV3" s="7">
+        <v>123</v>
+      </c>
+      <c r="CW3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="CZ3" s="9">
+        <v>1</v>
+      </c>
+      <c r="DA3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="DB3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC3" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD3" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="DE3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG3" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:111" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB4" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC4" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD4" s="1">
+        <v>6</v>
+      </c>
+      <c r="BE4" s="38" t="s">
+        <v>580</v>
+      </c>
+      <c r="BF4" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="BG4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI4" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK4" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL4" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM4" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="BN4" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO4" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BP4" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BQ4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="BR4" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS4" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="BU4" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BV4" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="BW4" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY4" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BZ4" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CA4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB4" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="CC4" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="CD4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE4" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="CG4" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH4" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CI4" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CJ4" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="CK4" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="CL4" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="CM4" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="CN4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="CO4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="CQ4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="CR4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CU4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV4" s="7">
+        <v>123</v>
+      </c>
+      <c r="CW4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="CZ4" s="9">
+        <v>1</v>
+      </c>
+      <c r="DA4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="DB4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC4" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD4" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="DE4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG4" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:111" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB5" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BE5" s="38" t="s">
+        <v>581</v>
+      </c>
+      <c r="BF5" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="BG5" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH5" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI5" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BJ5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL5" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM5" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="BN5" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO5" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BP5" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BQ5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS5" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BT5" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="BU5" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BV5" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="BW5" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="BX5" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY5" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BZ5" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CA5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB5" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="CC5" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE5" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="CF5" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="CG5" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH5" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CI5" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CJ5" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="CK5" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="CL5" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="CM5" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="CN5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="CO5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="CQ5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="CR5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CU5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV5" s="7">
+        <v>123</v>
+      </c>
+      <c r="CW5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="CZ5" s="9">
+        <v>1</v>
+      </c>
+      <c r="DA5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="DB5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC5" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD5" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="DE5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG5" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:111" ht="48" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU6" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="AZ6" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA6" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB6" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC6" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE6" s="38" t="s">
+        <v>582</v>
+      </c>
+      <c r="BF6" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="BG6" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH6" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI6" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK6" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL6" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM6" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="BN6" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO6" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BP6" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BQ6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="BR6" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS6" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BT6" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="BU6" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BV6" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="BW6" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="BX6" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY6" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BZ6" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CA6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB6" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="CC6" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="CD6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE6" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="CF6" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="CG6" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH6" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CI6" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CJ6" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="CK6" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="CL6" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="CM6" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="CN6" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="CO6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="CP6" s="7">
+        <v>345678</v>
+      </c>
+      <c r="CQ6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="CR6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="CS6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CU6" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV6" s="7">
+        <v>123</v>
+      </c>
+      <c r="CW6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="CZ6" s="9">
+        <v>1</v>
+      </c>
+      <c r="DA6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="DB6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC6" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD6" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="DE6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="DG6" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="45">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{25F60164-562A-48E3-8AC1-3D4314AA16B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R6" xr:uid="{25F60164-562A-48E3-8AC1-3D4314AA16B5}">
       <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{FB2E7975-C45A-4044-A09D-01478BE0CC22}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU6" xr:uid="{FB2E7975-C45A-4044-A09D-01478BE0CC22}">
       <formula1>"LCC,LCC+GDS,GDS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{D4A070FA-90F0-401D-86ED-16885515AA57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{D4A070FA-90F0-401D-86ED-16885515AA57}">
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{6C219D70-C84D-470D-91F5-D75280927F82}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{6C219D70-C84D-470D-91F5-D75280927F82}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{505A1FAB-445B-4B08-983E-70B20B60B500}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M6" xr:uid="{505A1FAB-445B-4B08-983E-70B20B60B500}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 DG2" xr:uid="{249F9713-76F2-4AC8-A20A-C618293667D2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6 DG2:DG6" xr:uid="{249F9713-76F2-4AC8-A20A-C618293667D2}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{C79C0E2B-0A1B-4D2A-8611-22A143F5AEF4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6" xr:uid="{C79C0E2B-0A1B-4D2A-8611-22A143F5AEF4}">
       <formula1>"Business trip  - Without reason"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{5E9A6754-E241-46E2-B2D3-ED802818109F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR6" xr:uid="{5E9A6754-E241-46E2-B2D3-ED802818109F}">
       <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{FADB8C77-ED57-4B66-9920-593FC152E36D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P6" xr:uid="{FADB8C77-ED57-4B66-9920-593FC152E36D}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2 AK2 AN2 DC2 CD2" xr:uid="{5E566F18-E6EF-40D8-91E5-BDA76AB29C03}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2:AP6 AK2:AK6 AN2:AN6 DC2:DC6 CD2:CD6" xr:uid="{5E566F18-E6EF-40D8-91E5-BDA76AB29C03}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DB2" xr:uid="{76FE0F58-E3FC-451E-9372-CF10DBD4D5A3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DB2:DB6" xr:uid="{76FE0F58-E3FC-451E-9372-CF10DBD4D5A3}">
       <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2" xr:uid="{CFEEC431-62CF-4087-A2D1-A5F9EDC2291E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2:CW6" xr:uid="{CFEEC431-62CF-4087-A2D1-A5F9EDC2291E}">
       <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{060E6A03-C224-4062-A54C-F69844C41AC3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6" xr:uid="{060E6A03-C224-4062-A54C-F69844C41AC3}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{86BE20C5-805B-4B6A-9B03-9C1026FF1459}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{86BE20C5-805B-4B6A-9B03-9C1026FF1459}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2 CY2 C2" xr:uid="{BC362102-86DA-491E-92AB-BB7399F63F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC6 CY2:CY6 C2:C6" xr:uid="{BC362102-86DA-491E-92AB-BB7399F63F17}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{E1DB1DAA-3729-49E6-A990-CAD6084A96CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O6" xr:uid="{E1DB1DAA-3729-49E6-A990-CAD6084A96CC}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{EB980B71-C557-4420-9F4E-8A2694C1CDA9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH6" xr:uid="{EB980B71-C557-4420-9F4E-8A2694C1CDA9}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{972F423D-F1D5-40DE-BC56-9CA1436471F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM6" xr:uid="{972F423D-F1D5-40DE-BC56-9CA1436471F0}">
       <formula1>"0,1,2,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU2" xr:uid="{DF49684E-C672-4142-BCEB-84EA90241E0B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU2:CU6" xr:uid="{DF49684E-C672-4142-BCEB-84EA90241E0B}">
       <formula1>"Master Card,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{6F3686EE-246B-4DB4-BB11-02C3EC33819F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S6" xr:uid="{6F3686EE-246B-4DB4-BB11-02C3EC33819F}">
       <formula1>"Individual,Guest,Personal,Dependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{DAD87662-E6E8-40DD-92C4-979C8552F30A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T6" xr:uid="{DAD87662-E6E8-40DD-92C4-979C8552F30A}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{7702B831-421E-4B60-9C57-C800F7B8A6D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U6" xr:uid="{7702B831-421E-4B60-9C57-C800F7B8A6D9}">
       <formula1>"OneWay,RoundTrip"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{3A64760F-D34B-4E60-AE36-BE71C7676729}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY6" xr:uid="{3A64760F-D34B-4E60-AE36-BE71C7676729}">
       <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel,Flight+MoreProducts"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 D2" xr:uid="{617A75F5-B873-470F-8224-2F5FA6AA66C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD6 D2:D6" xr:uid="{617A75F5-B873-470F-8224-2F5FA6AA66C3}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{546C0649-2FA6-49D3-AD11-F2EAD1C45578}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL6" xr:uid="{546C0649-2FA6-49D3-AD11-F2EAD1C45578}">
       <formula1>"InPolicy,OutPolicy,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{2AE44249-D30A-45F0-98EC-A8512DED6FDB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6" xr:uid="{2AE44249-D30A-45F0-98EC-A8512DED6FDB}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CR2" xr:uid="{FE062D84-BF61-47F5-BCBF-634752FF4142}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CR2:CR6" xr:uid="{FE062D84-BF61-47F5-BCBF-634752FF4142}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CS2" xr:uid="{D35036CE-2CFC-431F-9845-AEEF9CDC8F61}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CS2:CS6" xr:uid="{D35036CE-2CFC-431F-9845-AEEF9CDC8F61}">
       <formula1>"1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{FD4E3DD2-6FE5-4556-ACB9-7C3B3648902A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N6" xr:uid="{FD4E3DD2-6FE5-4556-ACB9-7C3B3648902A}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{BEE93905-D711-45DD-81F0-C3D752C20B57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT6" xr:uid="{BEE93905-D711-45DD-81F0-C3D752C20B57}">
       <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{AA58A214-4C3E-4476-8784-656901C29FE0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO6" xr:uid="{AA58A214-4C3E-4476-8784-656901C29FE0}">
       <formula1>"Duration,Layover,TimingFilter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{E0BA27C0-A15A-42BC-92AB-33294D8BE26D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{E0BA27C0-A15A-42BC-92AB-33294D8BE26D}">
       <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2" xr:uid="{E3516480-AA05-40A5-A4EF-9FF8B307E18F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2:CM6" xr:uid="{E3516480-AA05-40A5-A4EF-9FF8B307E18F}">
       <formula1>"Voter ID,Passport,PAN Card,Driving License"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2" xr:uid="{D1E8BD36-0F7A-4511-AA89-982206786A28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2:CL6" xr:uid="{D1E8BD36-0F7A-4511-AA89-982206786A28}">
       <formula1>"Male,Female,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CC2" xr:uid="{58295C26-370B-400F-9AA6-70F1CA9DB0FA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CC2:CC6" xr:uid="{58295C26-370B-400F-9AA6-70F1CA9DB0FA}">
       <formula1>"Excluding USA,Including USA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2" xr:uid="{EE4C5119-F37A-41B4-9AED-FBD1990A6BB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2:BZ6" xr:uid="{EE4C5119-F37A-41B4-9AED-FBD1990A6BB5}">
       <formula1>"Visitor,Tourist,Employment,Work Permit,Business,Student,Dependent,Work Permit Dependent,Family Visitor,Domestic Worker,Permanent Migration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2" xr:uid="{E1EAC2E4-4DA9-4183-8F17-944D9E3A9F2E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2:BY6" xr:uid="{E1EAC2E4-4DA9-4183-8F17-944D9E3A9F2E}">
       <formula1>"Bisht Travels [6683],Dilpreet.Singh [VBAll],Shaan_Test_Supplier [Shaan Quadlabs],Hertz Brazil [HZBR],Tourico [TOUR],AMERICAN AIRLINE [0012],MALAYSIA ARLN [232],Ashish [321],Hotel_Supplier [211287],Abacus Travels [555],GDS Travels [4567],Ashu Yadav [S007]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2" xr:uid="{30C26FFC-C1E3-4B0B-8703-EAAE9CA14974}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2:BX6" xr:uid="{30C26FFC-C1E3-4B0B-8703-EAAE9CA14974}">
       <formula1>"Transfers,Local Use,Outstation,Others "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2" xr:uid="{049682C2-ABA4-4775-BF8D-A16B874D1D7B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2:BW6" xr:uid="{049682C2-ABA4-4775-BF8D-A16B874D1D7B}">
       <formula1>"Sedan ,SUV,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2" xr:uid="{3CA2B307-A5B8-4518-8FF6-632EF08F0920}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2:BP6" xr:uid="{3CA2B307-A5B8-4518-8FF6-632EF08F0920}">
       <formula1>"Normal,Luxury"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{86EAD7DC-E70F-4E93-B604-F51E5DA283F5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2:BJ6" xr:uid="{86EAD7DC-E70F-4E93-B604-F51E5DA283F5}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2" xr:uid="{6A0A6352-E66F-433A-8737-8EDCF39606CD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2:BF6" xr:uid="{6A0A6352-E66F-433A-8737-8EDCF39606CD}">
       <formula1>"One Way,Round Trip,MultiCity"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2" xr:uid="{EAC7E2A2-7631-4CB0-8F65-2F1904825B22}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD6" xr:uid="{EAC7E2A2-7631-4CB0-8F65-2F1904825B22}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2" xr:uid="{6DE15265-BFDD-43D0-847F-CCE6BBA94AD5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2:BG6" xr:uid="{6DE15265-BFDD-43D0-847F-CCE6BBA94AD5}">
       <formula1>"Economy,Business,First,Premium Economy"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CI2" xr:uid="{81B33B7F-BBD0-46C9-B3C1-2DBD17E1C858}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CI6" xr:uid="{81B33B7F-BBD0-46C9-B3C1-2DBD17E1C858}">
       <formula1>"One Way,Round Trip"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19992,6 +21372,18 @@
     <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{ECEDCFC7-0E34-4131-B791-2108DA5D8FDE}"/>
     <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{59BA13CB-A0B3-4C25-9305-4D382065537B}"/>
     <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{C2C28B64-9E94-4C43-AEAA-6BF3B5C9590E}"/>
+    <hyperlink ref="N3" r:id="rId4" display="Admin@123" xr:uid="{C567EF04-1E6B-40E8-AAD7-C8514AE13D06}"/>
+    <hyperlink ref="I3" r:id="rId5" display="shekhar.singh@quadlabs.com" xr:uid="{F0C203AB-70F0-4535-B261-88BA97DFE0A3}"/>
+    <hyperlink ref="R3" r:id="rId6" display="ajit.kumar@quadlabs.com" xr:uid="{0BB79AF4-D5A8-4B91-902C-427D3E049F60}"/>
+    <hyperlink ref="N4" r:id="rId7" display="Admin@123" xr:uid="{B9FBD4D5-8AE9-4704-A5CA-BC76C033C145}"/>
+    <hyperlink ref="I4" r:id="rId8" display="shekhar.singh@quadlabs.com" xr:uid="{595DF3CB-710D-40A5-AC71-FFAF9352194E}"/>
+    <hyperlink ref="R4" r:id="rId9" display="ajit.kumar@quadlabs.com" xr:uid="{689E6AA1-4894-45FF-9DE9-85BBA751D46F}"/>
+    <hyperlink ref="N5" r:id="rId10" display="Admin@123" xr:uid="{6AB72D7A-CA6E-485D-92E5-BF010211E4F1}"/>
+    <hyperlink ref="I5" r:id="rId11" display="shekhar.singh@quadlabs.com" xr:uid="{C5579FC5-F9C2-4E0E-84B5-CA0E795C18E8}"/>
+    <hyperlink ref="R5" r:id="rId12" display="ajit.kumar@quadlabs.com" xr:uid="{EE827BEE-6781-47C8-BE75-266D14811B51}"/>
+    <hyperlink ref="N6" r:id="rId13" display="Admin@123" xr:uid="{0583D117-E598-4D19-B4AE-6392692ABFB1}"/>
+    <hyperlink ref="I6" r:id="rId14" display="shekhar.singh@quadlabs.com" xr:uid="{D2F07574-ED75-4262-92CF-A1B74C684168}"/>
+    <hyperlink ref="R6" r:id="rId15" display="ajit.kumar@quadlabs.com" xr:uid="{E184C77B-98F5-46FB-9886-188D7515573B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Shubham] Code on 4 June
</commit_message>
<xml_diff>
--- a/data/excel/FlightBookingWithMoreProducts.xlsx
+++ b/data/excel/FlightBookingWithMoreProducts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5BF1B3-45CB-4818-ADBA-6B385D72E1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC81197C-D2A5-4743-8743-953BA14A6A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -31,8 +31,9 @@
     <sheet name="Filtersheet" sheetId="91" r:id="rId16"/>
     <sheet name="Branding" sheetId="92" r:id="rId17"/>
     <sheet name="Sheet11" sheetId="97" r:id="rId18"/>
-    <sheet name="NonBranding" sheetId="96" r:id="rId19"/>
-    <sheet name="Sheet17" sheetId="95" r:id="rId20"/>
+    <sheet name="Sheet15" sheetId="98" r:id="rId19"/>
+    <sheet name="NonBranding" sheetId="96" r:id="rId20"/>
+    <sheet name="Sheet17" sheetId="95" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8888" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9093" uniqueCount="590">
   <si>
     <t>del</t>
   </si>
@@ -1819,6 +1820,12 @@
   </si>
   <si>
     <t>Verify on Add to Cart with adding 3 more products for Flight booking.</t>
+  </si>
+  <si>
+    <t>29-Aug-2024</t>
+  </si>
+  <si>
+    <t>13-Aug-2024</t>
   </si>
 </sst>
 </file>
@@ -19101,8 +19108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1152101-88D1-47D8-974F-BB578AD00182}">
   <dimension ref="A1:DG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21390,17 +21397,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B5143E-7EC1-42F1-ACFE-7B1A3D040ECA}">
-  <dimension ref="A1:BW7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA22B64-135C-4D3B-9A16-80CCFF03F711}">
+  <dimension ref="A1:DG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
@@ -21415,17 +21422,17 @@
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="36" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -21448,34 +21455,70 @@
     <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="17" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="14" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="9" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>35</v>
       </c>
@@ -21641,73 +21684,181 @@
       <c r="BC1" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="BD1" s="23" t="s">
+      <c r="BD1" s="24" t="s">
+        <v>520</v>
+      </c>
+      <c r="BE1" s="37" t="s">
+        <v>521</v>
+      </c>
+      <c r="BF1" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="BG1" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="BH1" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="BI1" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="BJ1" s="24" t="s">
+        <v>526</v>
+      </c>
+      <c r="BK1" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="BL1" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="BM1" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="BN1" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="BO1" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="BP1" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="BQ1" s="24" t="s">
+        <v>533</v>
+      </c>
+      <c r="BR1" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="BS1" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="BT1" s="24" t="s">
+        <v>536</v>
+      </c>
+      <c r="BU1" s="24" t="s">
+        <v>537</v>
+      </c>
+      <c r="BV1" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="BW1" s="24" t="s">
+        <v>539</v>
+      </c>
+      <c r="BX1" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="BY1" s="24" t="s">
+        <v>541</v>
+      </c>
+      <c r="BZ1" s="24" t="s">
+        <v>542</v>
+      </c>
+      <c r="CA1" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="CB1" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="CC1" s="24" t="s">
+        <v>545</v>
+      </c>
+      <c r="CD1" s="24" t="s">
+        <v>546</v>
+      </c>
+      <c r="CE1" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="CF1" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="CG1" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="CH1" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="CI1" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="CJ1" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="CK1" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="CL1" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="CM1" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="CN1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="BE1" s="23" t="s">
+      <c r="CO1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="BF1" s="23" t="s">
+      <c r="CP1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="BG1" s="23" t="s">
+      <c r="CQ1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="BH1" s="23" t="s">
+      <c r="CR1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="BI1" s="14" t="s">
+      <c r="CS1" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="BJ1" s="14" t="s">
+      <c r="CT1" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="BK1" s="23" t="s">
+      <c r="CU1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="BL1" s="23" t="s">
+      <c r="CV1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="BM1" s="23" t="s">
+      <c r="CW1" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="BN1" s="23" t="s">
+      <c r="CX1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="BO1" s="19" t="s">
+      <c r="CY1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="19" t="s">
+      <c r="CZ1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="19" t="s">
+      <c r="DA1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="23" t="s">
+      <c r="DB1" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="BS1" s="23" t="s">
+      <c r="DC1" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="BT1" s="23" t="s">
+      <c r="DD1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="BU1" s="23" t="s">
+      <c r="DE1" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="BV1" s="23" t="s">
+      <c r="DF1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BW1" s="23" t="s">
+      <c r="DG1" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:111" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>500</v>
+        <v>583</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>56</v>
@@ -21728,13 +21879,13 @@
         <v>403</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>442</v>
+        <v>343</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>408</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>52</v>
@@ -21749,13 +21900,13 @@
         <v>59</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>444</v>
+        <v>192</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>445</v>
+        <v>293</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>459</v>
+        <v>343</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>32</v>
@@ -21764,7 +21915,7 @@
         <v>132</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>337</v>
+        <v>137</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>448</v>
@@ -21772,20 +21923,20 @@
       <c r="W2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="X2" s="36" t="s">
-        <v>449</v>
+      <c r="X2" s="7" t="s">
+        <v>484</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>485</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="30" t="s">
         <v>246</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>495</v>
+        <v>589</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>511</v>
+        <v>588</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>69</v>
@@ -21830,10 +21981,10 @@
         <v>153</v>
       </c>
       <c r="AQ2" s="7" t="s">
-        <v>353</v>
+        <v>139</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>353</v>
+        <v>139</v>
       </c>
       <c r="AS2" s="13" t="s">
         <v>292</v>
@@ -21854,7 +22005,7 @@
         <v>1</v>
       </c>
       <c r="AY2" s="7" t="s">
-        <v>70</v>
+        <v>574</v>
       </c>
       <c r="AZ2" s="13" t="s">
         <v>140</v>
@@ -21868,1313 +22019,317 @@
       <c r="BC2" s="34" t="s">
         <v>476</v>
       </c>
-      <c r="BD2" s="7">
+      <c r="BD2" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE2" s="38" t="s">
+        <v>556</v>
+      </c>
+      <c r="BF2" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="BG2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BT2" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="BY2" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BZ2" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CA2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB2" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="CC2" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="CD2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE2" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="CF2" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="CK2" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="CL2" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="CM2" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="CN2" s="7">
         <v>78554432323</v>
       </c>
-      <c r="BE2" s="7" t="s">
+      <c r="CO2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="BF2" s="7">
+      <c r="CP2" s="7">
         <v>345678</v>
       </c>
-      <c r="BG2" s="7" t="s">
+      <c r="CQ2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="BH2" s="7" t="s">
+      <c r="CR2" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="BI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="CS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BK2" s="7" t="s">
+      <c r="CU2" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="BL2" s="7">
+      <c r="CV2" s="7">
         <v>123</v>
       </c>
-      <c r="BM2" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN2" s="7" t="s">
+      <c r="CW2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="BO2" s="9" t="s">
+      <c r="CY2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="BP2" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ2" s="9" t="s">
+      <c r="CZ2" s="9">
+        <v>1</v>
+      </c>
+      <c r="DA2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="BR2" s="7" t="s">
+      <c r="DB2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="BS2" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT2" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU2" s="7" t="s">
+      <c r="DC2" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD2" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="DE2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BV2" s="7" t="s">
+      <c r="DF2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="BW2" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:75" ht="48" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>517</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R3" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z3" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>518</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK3" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO3" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AP3" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ3" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR3" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AS3" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AT3" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AU3" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="AV3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AY3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ3" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA3" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB3" s="34" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC3" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="BD3" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="BE3" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF3" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BG3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BH3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BK3" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BL3" s="7">
-        <v>123</v>
-      </c>
-      <c r="BM3" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP3" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BR3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS3" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT3" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BV3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BW3" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="4" spans="1:75" ht="48" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R4" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="Z4" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>507</v>
-      </c>
-      <c r="AB4" s="12" t="s">
-        <v>512</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO4" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AP4" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR4" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="AS4" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AT4" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="AU4" s="13" t="s">
-        <v>499</v>
-      </c>
-      <c r="AV4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AY4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ4" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA4" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB4" s="34" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC4" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="BD4" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="BE4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF4" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BG4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BH4" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI4" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BK4" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BL4" s="7">
-        <v>123</v>
-      </c>
-      <c r="BM4" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP4" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BR4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS4" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT4" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU4" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BV4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BW4" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="5" spans="1:75" ht="48" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R5" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z5" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA5" s="12" t="s">
-        <v>509</v>
-      </c>
-      <c r="AB5" s="12" t="s">
-        <v>514</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE5" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK5" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO5" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AP5" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ5" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="AR5" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="AS5" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="AT5" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="AU5" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="AV5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AY5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ5" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA5" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB5" s="34" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC5" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="BD5" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="BE5" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF5" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BG5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BH5" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI5" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BK5" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BL5" s="7">
-        <v>123</v>
-      </c>
-      <c r="BM5" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP5" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BR5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS5" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT5" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BV5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BW5" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="6" spans="1:75" ht="48" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R6" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="Z6" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA6" s="12" t="s">
-        <v>510</v>
-      </c>
-      <c r="AB6" s="12" t="s">
-        <v>515</v>
-      </c>
-      <c r="AC6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD6" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE6" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK6" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO6" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AP6" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ6" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="AR6" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="AS6" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AT6" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AU6" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="AV6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX6" s="7">
-        <v>1</v>
-      </c>
-      <c r="AY6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ6" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA6" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB6" s="34" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC6" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="BD6" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="BE6" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF6" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BG6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BH6" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI6" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BK6" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BL6" s="7">
-        <v>123</v>
-      </c>
-      <c r="BM6" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP6" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BR6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS6" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT6" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU6" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BV6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BW6" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="7" spans="1:75" ht="48" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R7" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="X7" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="Z7" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>516</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>509</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD7" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF7" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK7" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="AO7" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AP7" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ7" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="AR7" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="AS7" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="AT7" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="AU7" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="AV7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AY7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ7" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BA7" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB7" s="34" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC7" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="BD7" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="BE7" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF7" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BG7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BH7" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="BI7" s="1">
-        <v>1</v>
-      </c>
-      <c r="BJ7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BK7" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BL7" s="7">
-        <v>123</v>
-      </c>
-      <c r="BM7" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="BN7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP7" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BR7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS7" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BT7" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU7" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BV7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BW7" s="7" t="s">
-        <v>443</v>
+      <c r="DG2" s="7" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="32">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R7" xr:uid="{D024D7FF-5877-417E-8C21-AC9B5D1F8CA7}">
+  <dataValidations count="45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CI2" xr:uid="{B185E19D-5531-4502-8FEC-CB5BF96E63F6}">
+      <formula1>"One Way,Round Trip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2" xr:uid="{8AE27B0E-545E-407B-A353-FEFFBB9A451C}">
+      <formula1>"Economy,Business,First,Premium Economy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2" xr:uid="{CD2A0CB3-1625-4C77-804E-0BEDD3F6684C}">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2" xr:uid="{6D7CB7DD-5857-4683-B44F-DBC993100363}">
+      <formula1>"One Way,Round Trip,MultiCity"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{5A2E32C9-D4B7-49C9-BDE0-2E47147A576F}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2" xr:uid="{BC4354E8-39A3-4012-BC4B-4A9D3C69BF08}">
+      <formula1>"Normal,Luxury"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BW2" xr:uid="{0D56F12A-28F1-4DC6-859A-CFA67C90669C}">
+      <formula1>"Sedan ,SUV,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2" xr:uid="{1518C4AD-9352-4B4F-85DD-84EC4B5EC781}">
+      <formula1>"Transfers,Local Use,Outstation,Others "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2" xr:uid="{97C5D3E4-0F75-4CDA-998A-EF2CF76844EA}">
+      <formula1>"Bisht Travels [6683],Dilpreet.Singh [VBAll],Shaan_Test_Supplier [Shaan Quadlabs],Hertz Brazil [HZBR],Tourico [TOUR],AMERICAN AIRLINE [0012],MALAYSIA ARLN [232],Ashish [321],Hotel_Supplier [211287],Abacus Travels [555],GDS Travels [4567],Ashu Yadav [S007]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2" xr:uid="{095A30FB-9551-47B5-864C-6689F403D280}">
+      <formula1>"Visitor,Tourist,Employment,Work Permit,Business,Student,Dependent,Work Permit Dependent,Family Visitor,Domestic Worker,Permanent Migration"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CC2" xr:uid="{02E9CDFC-BD05-4260-B064-8F70AE03C786}">
+      <formula1>"Excluding USA,Including USA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2" xr:uid="{BE7364D3-6886-4FDC-98E0-F1EA97A801F0}">
+      <formula1>"Male,Female,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2" xr:uid="{419DD657-E6DB-40C3-8D77-E81CBCE99B73}">
+      <formula1>"Voter ID,Passport,PAN Card,Driving License"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{77C0E26D-84C6-4681-9C0E-E575789CE449}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{BA53B031-D995-4B2F-9E5B-6B4BAA8DD710}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{1D3F0CB6-0CF1-4854-A43C-5CA83CEC7703}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{6E1684F4-3EFC-44B0-B9C1-262CE35A176D}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CS2" xr:uid="{6CA63AB0-9514-47E6-966B-D9854CF172DE}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CR2" xr:uid="{33223260-14B7-4D7A-B7C7-78443AE15F14}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{F27C043E-BCF0-4AF1-B1BA-1E9A82A7C3C0}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{E076AF52-F8F9-44D8-9997-D6D69D045A57}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 D2" xr:uid="{EB3FEE0A-BF35-4020-A481-14F103FA2806}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{887943BC-E92B-4209-B1FA-F2B3ADFC9D9D}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel,Flight+MoreProducts"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{A04F6E50-4532-4277-9A04-8362A4EA3111}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{3A98737D-5C7A-4067-8591-860B44395E7C}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{D21EEC15-BD3F-4337-BF19-5016D29A13F7}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU2" xr:uid="{32786FBD-AAAF-441B-9C53-47B5B60A922E}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{6A0AA00B-59EB-4D5D-80FF-DD004E05C1F6}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{C960591F-D654-4B6F-8C62-94AFE0C729CB}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{C84C1AD7-D1F4-4577-8843-FB6043005E7B}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2 CY2 C2" xr:uid="{D7470D76-5E30-47F2-B2F5-DB9FFA0576CD}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{3487237B-1529-436F-AB51-F826610F89B6}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{8456843C-A835-47C2-BF21-4B35B607EE80}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2" xr:uid="{E9E7535C-013D-4460-B6C9-59EB00A49A21}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DB2" xr:uid="{C2F72938-C2D5-4BEB-9594-B3AE18D1CE0F}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2 AK2 AN2 DC2 CD2" xr:uid="{CC759BF9-11AF-4BBD-A9E9-9D8DB2A117BE}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{5CF567A3-8D5C-4919-803C-C72C0776EB59}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{7987ED9D-23B5-44F2-8235-9D08F86B2A17}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{24E2A86B-3B66-4BF1-8C3A-45732797F06B}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 DG2" xr:uid="{717B18CD-263C-4788-AEE7-D32388F29479}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{BDC08B0A-4245-47B9-AC49-47AE12BAC8A4}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{7F4EC7E1-2B36-4D3A-9553-593EF9B7B4F3}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{9D35340B-A1C7-42E2-95AD-179456A27B7C}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{7EDDBFCC-DD85-4BAB-8023-1652E83B6BD8}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{45D331DC-3677-4D9B-B9D4-97E1506A904B}">
       <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU7" xr:uid="{4C2EDD49-F03F-44BA-B1B8-0C136E083675}">
-      <formula1>"LCC,LCC+GDS,GDS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{23A46B36-DA52-4C07-895C-BE6A8632AE14}">
-      <formula1>"Normal,SSO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{068909F9-1BBD-41F4-8849-032AB66C945E}">
-      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{76AB454B-9E0E-4A0C-8699-6A5D118E1C80}">
-      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7 BW2:BW7" xr:uid="{5B655824-089E-4155-A471-2E4B953D4352}">
-      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z7" xr:uid="{E6CF0F22-524C-4672-9F14-15C0D88E8F5B}">
-      <formula1>"Business trip  - Without reason"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR7" xr:uid="{1979A165-151B-4A1C-A673-EA35B65C343E}">
-      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P7" xr:uid="{9BFD1C69-9188-48AC-A569-3C49A29B4462}">
-      <formula1>"On,Off"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2:BS7 AN2:AN7 AK2:AK7 AP2:AP7" xr:uid="{193811A6-9F52-4E9A-8B76-B07D9E985177}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR7" xr:uid="{1BDB8AF6-EF2C-4961-9DFE-57A3DEADACBA}">
-      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM7" xr:uid="{59EEE077-0DA6-4262-8C44-9A7B7BA8C20B}">
-      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7" xr:uid="{AFEEE849-A3D6-4969-BD6A-44189286F05D}">
-      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7" xr:uid="{6FCF972E-7DCD-4529-A74B-20A98452F1CC}">
-      <formula1>"sbt,preprod117"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7 BO2:BO7 AC2:AC7" xr:uid="{9AE4D64B-6BB3-4B65-9210-7D14B8E279BF}">
-      <formula1>"Applied,NotApplied"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O7" xr:uid="{E7E93449-81F1-437E-9466-FCAE3EB13B34}">
-      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH7" xr:uid="{57C1CD49-D81E-4CDA-ADC2-333E298D6DD0}">
-      <formula1>"0,1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM7" xr:uid="{0127F8DA-9C08-45CD-8FAD-0FC6A9948873}">
-      <formula1>"0,1,2,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK7" xr:uid="{C3ADB87A-3DAF-43D2-B61E-6A59AC77244F}">
-      <formula1>"Master Card,Visa"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S7" xr:uid="{10D74546-3B89-4934-BAAC-ADACDD978C07}">
-      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T7" xr:uid="{3BCB5532-36B1-4688-BCF7-AB2BDF21ABD4}">
-      <formula1>"Domestic,International"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U7" xr:uid="{D7F0DC9D-3959-4718-B297-E9ECED9A0DD7}">
-      <formula1>"OneWay,RoundTrip"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY7" xr:uid="{0CA3DD45-8728-4DAC-8734-22AAE78A4C44}">
-      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 AD2:AD7" xr:uid="{70CB9E9E-DC29-424B-A299-C70286D5C8A3}">
-      <formula1>"1,2,3,4,5,6,7,8"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7" xr:uid="{4ABB4FC5-3500-4E6F-AEBA-AD8C6A7B4B2C}">
-      <formula1>"InPolicy,OutPolicy,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q7" xr:uid="{F4DEB8CA-EC4B-48AA-BB77-81A22662FE0E}">
-      <formula1>"Old,New"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH7" xr:uid="{5A8206FF-C0CF-4DB1-BC6D-021DB9E7D33C}">
-      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI7" xr:uid="{5ADD087C-10E9-4870-A4C5-C6A8DCE3887B}">
-      <formula1>"1,2,3,4,5,6"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N7" xr:uid="{0C07B452-AE94-4F16-8DF4-58EBCD080F04}">
-      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT7" xr:uid="{2B5D6E92-6B4E-4398-9FB0-ECA48C538D48}">
-      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO7" xr:uid="{0CF9A97E-6EE1-403B-BC9D-2B189D56E156}">
-      <formula1>"Duration,Layover,TimingFilter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7" xr:uid="{BA6EB1E2-9966-4D56-8CCD-47062AABC97D}">
-      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{36741546-A047-41F4-8FD6-332B511AC497}"/>
-    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{52C22434-0242-4BA0-8214-10A45065AA6D}"/>
-    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{B6437C01-074E-4F66-8471-605B892771AA}"/>
-    <hyperlink ref="N4" r:id="rId4" display="Admin@123" xr:uid="{6E97E840-FFAF-43A0-A061-487737F951DB}"/>
-    <hyperlink ref="N6" r:id="rId5" display="Admin@123" xr:uid="{EE183E74-5766-44BC-AC1F-E8D6BCC0BBCB}"/>
-    <hyperlink ref="N7" r:id="rId6" display="Admin@123" xr:uid="{A309F605-A086-45B9-8FD8-5A999C33AD94}"/>
-    <hyperlink ref="N5" r:id="rId7" display="Admin@123" xr:uid="{EBE27E5A-247F-4972-9E49-AE8F4A8D2739}"/>
-    <hyperlink ref="N3" r:id="rId8" display="Admin@123" xr:uid="{2CCAC76D-2183-4AD6-B662-7675D4BAB0B5}"/>
-    <hyperlink ref="I3:I7" r:id="rId9" display="shekhar.singh@quadlabs.com" xr:uid="{4DEAAFA1-B1F8-4B52-89F8-D5A367DCAA50}"/>
-    <hyperlink ref="R3:R7" r:id="rId10" display="ajit.kumar@quadlabs.com" xr:uid="{9FB03654-ED91-46F9-B963-7460745D3E8B}"/>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{67116AD2-C826-4F46-A707-85CE0CCD65C0}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{9BF81C11-6BC4-4FE7-B5EE-DD12ADA88B11}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{580BA13A-4B44-4CBE-BBFF-4F116B1DC9B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24361,10 +23516,1801 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B5143E-7EC1-42F1-ACFE-7B1A3D040ECA}">
+  <dimension ref="A1:BW7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X2" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC2" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS2" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB3" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC3" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB4" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC4" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL4" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS4" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW4" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB5" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL5" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP5" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS5" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT5" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW5" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z6" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT6" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU6" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ6" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA6" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB6" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC6" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD6" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF6" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK6" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL6" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM6" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP6" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS6" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT6" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW6" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R7" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z7" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK7" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO7" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ7" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR7" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS7" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AT7" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AU7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ7" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA7" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB7" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC7" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD7" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF7" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH7" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK7" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL7" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM7" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="BN7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP7" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS7" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT7" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW7" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R7" xr:uid="{D024D7FF-5877-417E-8C21-AC9B5D1F8CA7}">
+      <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU7" xr:uid="{4C2EDD49-F03F-44BA-B1B8-0C136E083675}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{23A46B36-DA52-4C07-895C-BE6A8632AE14}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{068909F9-1BBD-41F4-8849-032AB66C945E}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{76AB454B-9E0E-4A0C-8699-6A5D118E1C80}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7 BW2:BW7" xr:uid="{5B655824-089E-4155-A471-2E4B953D4352}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z7" xr:uid="{E6CF0F22-524C-4672-9F14-15C0D88E8F5B}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR7" xr:uid="{1979A165-151B-4A1C-A673-EA35B65C343E}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P7" xr:uid="{9BFD1C69-9188-48AC-A569-3C49A29B4462}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2:BS7 AN2:AN7 AK2:AK7 AP2:AP7" xr:uid="{193811A6-9F52-4E9A-8B76-B07D9E985177}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR7" xr:uid="{1BDB8AF6-EF2C-4961-9DFE-57A3DEADACBA}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM7" xr:uid="{59EEE077-0DA6-4262-8C44-9A7B7BA8C20B}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L7" xr:uid="{AFEEE849-A3D6-4969-BD6A-44189286F05D}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7" xr:uid="{6FCF972E-7DCD-4529-A74B-20A98452F1CC}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7 BO2:BO7 AC2:AC7" xr:uid="{9AE4D64B-6BB3-4B65-9210-7D14B8E279BF}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O7" xr:uid="{E7E93449-81F1-437E-9466-FCAE3EB13B34}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH7" xr:uid="{57C1CD49-D81E-4CDA-ADC2-333E298D6DD0}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM7" xr:uid="{0127F8DA-9C08-45CD-8FAD-0FC6A9948873}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK7" xr:uid="{C3ADB87A-3DAF-43D2-B61E-6A59AC77244F}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S7" xr:uid="{10D74546-3B89-4934-BAAC-ADACDD978C07}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T7" xr:uid="{3BCB5532-36B1-4688-BCF7-AB2BDF21ABD4}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U7" xr:uid="{D7F0DC9D-3959-4718-B297-E9ECED9A0DD7}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY7" xr:uid="{0CA3DD45-8728-4DAC-8734-22AAE78A4C44}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7 AD2:AD7" xr:uid="{70CB9E9E-DC29-424B-A299-C70286D5C8A3}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7" xr:uid="{4ABB4FC5-3500-4E6F-AEBA-AD8C6A7B4B2C}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q7" xr:uid="{F4DEB8CA-EC4B-48AA-BB77-81A22662FE0E}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH7" xr:uid="{5A8206FF-C0CF-4DB1-BC6D-021DB9E7D33C}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI7" xr:uid="{5ADD087C-10E9-4870-A4C5-C6A8DCE3887B}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N7" xr:uid="{0C07B452-AE94-4F16-8DF4-58EBCD080F04}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT7" xr:uid="{2B5D6E92-6B4E-4398-9FB0-ECA48C538D48}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO7" xr:uid="{0CF9A97E-6EE1-403B-BC9D-2B189D56E156}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I7" xr:uid="{BA6EB1E2-9966-4D56-8CCD-47062AABC97D}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{36741546-A047-41F4-8FD6-332B511AC497}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{52C22434-0242-4BA0-8214-10A45065AA6D}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{B6437C01-074E-4F66-8471-605B892771AA}"/>
+    <hyperlink ref="N4" r:id="rId4" display="Admin@123" xr:uid="{6E97E840-FFAF-43A0-A061-487737F951DB}"/>
+    <hyperlink ref="N6" r:id="rId5" display="Admin@123" xr:uid="{EE183E74-5766-44BC-AC1F-E8D6BCC0BBCB}"/>
+    <hyperlink ref="N7" r:id="rId6" display="Admin@123" xr:uid="{A309F605-A086-45B9-8FD8-5A999C33AD94}"/>
+    <hyperlink ref="N5" r:id="rId7" display="Admin@123" xr:uid="{EBE27E5A-247F-4972-9E49-AE8F4A8D2739}"/>
+    <hyperlink ref="N3" r:id="rId8" display="Admin@123" xr:uid="{2CCAC76D-2183-4AD6-B662-7675D4BAB0B5}"/>
+    <hyperlink ref="I3:I7" r:id="rId9" display="shekhar.singh@quadlabs.com" xr:uid="{4DEAAFA1-B1F8-4B52-89F8-D5A367DCAA50}"/>
+    <hyperlink ref="R3:R7" r:id="rId10" display="ajit.kumar@quadlabs.com" xr:uid="{9FB03654-ED91-46F9-B963-7460745D3E8B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4DC434-9680-44B9-B67E-2B0017A95C76}">
   <dimension ref="A1:BW2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Shubham] Push code with new functionality
</commit_message>
<xml_diff>
--- a/data/excel/FlightBookingWithMoreProducts.xlsx
+++ b/data/excel/FlightBookingWithMoreProducts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143E1333-F896-48CC-AD19-CDD2D1ABA2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A95F48-0C95-476E-90B2-98F2A01A0C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21483,8 +21483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA22B64-135C-4D3B-9A16-80CCFF03F711}">
   <dimension ref="A1:DG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>